<commit_message>
excel without polish letters
</commit_message>
<xml_diff>
--- a/DaneHelwig.xlsx
+++ b/DaneHelwig.xlsx
@@ -59,9 +59,6 @@
     <t>Przeciętne miesięczne wynagrodzenia brutto w zł</t>
   </si>
   <si>
-    <t>Dolnośląskie</t>
-  </si>
-  <si>
     <t>Kujawsko-pomorskie</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
     <t>Lubuskie</t>
   </si>
   <si>
-    <t>Łódzkie</t>
-  </si>
-  <si>
-    <t>Małopolskie</t>
-  </si>
-  <si>
     <t>Mazowieckie</t>
   </si>
   <si>
@@ -92,15 +83,6 @@
     <t>Pomorskie</t>
   </si>
   <si>
-    <t>Śląskie</t>
-  </si>
-  <si>
-    <t>Świętokrzyskie</t>
-  </si>
-  <si>
-    <t>Warmińsko-mazurskie</t>
-  </si>
-  <si>
     <t>Wielkopolskie</t>
   </si>
   <si>
@@ -156,6 +138,24 @@
   </si>
   <si>
     <t>Zdrowie</t>
+  </si>
+  <si>
+    <t>Dolnoslaskie</t>
+  </si>
+  <si>
+    <t>Lodzkie</t>
+  </si>
+  <si>
+    <t>Malopolskie</t>
+  </si>
+  <si>
+    <t>Slaskie</t>
+  </si>
+  <si>
+    <t>Swietokrzyskie</t>
+  </si>
+  <si>
+    <t>Warminsko-mazurskie</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,51 +592,51 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2">
         <v>2550.6999999999998</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2">
         <v>1924.8</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
         <v>1996</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2">
         <v>3347.6</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2">
         <v>4015.7</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2">
         <v>3596.2</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>5719.7</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>3565.6</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
         <v>1806.5</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
         <v>1251.5</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>2689.8</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2">
         <v>3994.6</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2">
         <v>1598.7</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2">
         <v>2956.1</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>1995.3</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2">
         <v>1195.7</v>
@@ -1430,46 +1430,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1518,90 +1518,90 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>